<commit_message>
Develop City, District & Village
</commit_message>
<xml_diff>
--- a/Countries.xlsx
+++ b/Countries.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -28,13 +28,13 @@
     <t>Icon Flag Path</t>
   </si>
   <si>
-    <t>4410d3f6-d600-42b5-a43b-7c117b214119</t>
-  </si>
-  <si>
-    <t>Indonesias</t>
-  </si>
-  <si>
-    <t>+623</t>
+    <t>21f66d32-6a6f-482f-88cb-2a3657251185</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>+62</t>
   </si>
   <si>
     <t/>
@@ -46,7 +46,13 @@
     <t>Jepang</t>
   </si>
   <si>
-    <t>+62</t>
+    <t>7f7de98c-755e-46cc-ac65-cbf96b2204de</t>
+  </si>
+  <si>
+    <t>Malasya</t>
+  </si>
+  <si>
+    <t>+63</t>
   </si>
 </sst>
 </file>
@@ -357,7 +363,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col customWidth="true" max="1" min="1" width="38"/>
-    <col customWidth="true" max="3" min="2" width="12"/>
+    <col customWidth="true" max="2" min="2" width="11"/>
+    <col customWidth="true" max="3" min="3" width="12"/>
     <col customWidth="true" max="4" min="4" width="16"/>
   </cols>
   <sheetData>
@@ -397,9 +404,23 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>